<commit_message>
office Copy - 22-9-21
</commit_message>
<xml_diff>
--- a/Daily Work Pc.xlsx
+++ b/Daily Work Pc.xlsx
@@ -15,8 +15,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <authors>
+    <author>Author</author>
+  </authors>
+  <commentList>
+    <comment ref="D5" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+16-09-21 to 21-09-21</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="14">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="17">
   <si>
     <t>Stock Entry Delivery &amp; Received</t>
   </si>
@@ -42,9 +76,6 @@
     <t>Program  Wise Delivery Challan Entry</t>
   </si>
   <si>
-    <t>4 Dayes</t>
-  </si>
-  <si>
     <t>Reporting Date</t>
   </si>
   <si>
@@ -58,13 +89,25 @@
   </si>
   <si>
     <t>21.09.21</t>
+  </si>
+  <si>
+    <t>6 Dayes</t>
+  </si>
+  <si>
+    <t>Issue Pending</t>
+  </si>
+  <si>
+    <t>20-09-21</t>
+  </si>
+  <si>
+    <t>21-09-21</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -108,6 +151,19 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -501,11 +557,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:F8"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A2:G8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -518,7 +574,7 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:6" ht="23.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="23.25" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>4</v>
       </c>
@@ -526,33 +582,33 @@
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
     </row>
-    <row r="3" spans="1:6" ht="21" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" ht="21" x14ac:dyDescent="0.25">
       <c r="B3" s="2"/>
       <c r="C3" s="4"/>
       <c r="D3" s="5"/>
       <c r="E3" s="5" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3"/>
       <c r="B4" s="3" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="3"/>
       <c r="B5" s="3" t="s">
         <v>1</v>
@@ -561,34 +617,43 @@
         <v>3</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>8</v>
+        <v>13</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="3"/>
       <c r="B6" s="3" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3"/>
       <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>3</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="18.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="18.75" x14ac:dyDescent="0.25">
       <c r="A8" s="3"/>
       <c r="B8" s="3" t="s">
         <v>6</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>5</v>
@@ -629,6 +694,7 @@
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
 

</xml_diff>